<commit_message>
Updated Cantus Firmus Graphs
</commit_message>
<xml_diff>
--- a/analysis/op_art_analysis.xlsx
+++ b/analysis/op_art_analysis.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hettysymes/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hettysymes/PycharmProjects/op_art_generator/analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9E82A00A-E6F5-7E43-925C-9837E4AC9E97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A13E25F3-FF47-9C45-8CFE-DF42E2F42AC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16100" activeTab="2" xr2:uid="{F32E88F0-E047-FC4B-8F82-E7C145B1565C}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16080" activeTab="3" xr2:uid="{F32E88F0-E047-FC4B-8F82-E7C145B1565C}"/>
   </bookViews>
   <sheets>
     <sheet name="Carnival " sheetId="10" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="155">
   <si>
     <t>Index</t>
   </si>
@@ -323,9 +323,6 @@
     <t>black</t>
   </si>
   <si>
-    <t>grey</t>
-  </si>
-  <si>
     <t>white</t>
   </si>
   <si>
@@ -495,6 +492,24 @@
   </si>
   <si>
     <t>curvature_abs</t>
+  </si>
+  <si>
+    <t>grey1</t>
+  </si>
+  <si>
+    <t>grey2</t>
+  </si>
+  <si>
+    <t>grey3</t>
+  </si>
+  <si>
+    <t>grey4</t>
+  </si>
+  <si>
+    <t>grey5</t>
+  </si>
+  <si>
+    <t>grey6</t>
   </si>
 </sst>
 </file>
@@ -27167,10 +27182,10 @@
         <v>94.72</v>
       </c>
       <c r="G1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="J1" t="s">
         <v>25</v>
@@ -27187,10 +27202,10 @@
         <v>252.45</v>
       </c>
       <c r="G2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="J2" t="s">
         <v>27</v>
@@ -27201,10 +27216,10 @@
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="G3" t="s">
+        <v>120</v>
+      </c>
+      <c r="H3" t="s">
         <v>121</v>
-      </c>
-      <c r="H3" t="s">
-        <v>122</v>
       </c>
       <c r="K3">
         <f>K1/K2</f>
@@ -27229,12 +27244,12 @@
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="E6" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="E8" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F8">
         <v>48.49</v>
@@ -27243,7 +27258,7 @@
         <v>45.55</v>
       </c>
       <c r="I8" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="J8">
         <f>(G9-G8)/2</f>
@@ -27263,7 +27278,7 @@
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.2">
       <c r="E9" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F9">
         <v>191.03</v>
@@ -27272,7 +27287,7 @@
         <v>89.64</v>
       </c>
       <c r="I9" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="J9">
         <f>(F9-F8)*2</f>
@@ -27298,7 +27313,7 @@
         <v>78.58</v>
       </c>
       <c r="I11" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="J11">
         <f>F8-F11</f>
@@ -27325,7 +27340,7 @@
         <v>124.47</v>
       </c>
       <c r="I12" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="J12">
         <f>G11-G8</f>
@@ -27346,7 +27361,7 @@
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B15">
         <v>194.18</v>
@@ -28262,25 +28277,25 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B1" t="s">
+        <v>132</v>
+      </c>
+      <c r="C1" t="s">
         <v>133</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>134</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>135</v>
-      </c>
-      <c r="E1" t="s">
-        <v>136</v>
       </c>
       <c r="F1" t="s">
         <v>57</v>
       </c>
       <c r="G1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="M1" t="s">
         <v>25</v>
@@ -28560,46 +28575,46 @@
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
+        <v>136</v>
+      </c>
+      <c r="B16" t="s">
         <v>137</v>
       </c>
-      <c r="B16" t="s">
+      <c r="C16" t="s">
         <v>138</v>
       </c>
-      <c r="C16" t="s">
+      <c r="D16" t="s">
         <v>139</v>
       </c>
-      <c r="D16" t="s">
+      <c r="E16" t="s">
         <v>140</v>
-      </c>
-      <c r="E16" t="s">
-        <v>141</v>
       </c>
       <c r="F16" t="s">
         <v>27</v>
       </c>
       <c r="G16" t="s">
+        <v>141</v>
+      </c>
+      <c r="H16" t="s">
         <v>142</v>
-      </c>
-      <c r="H16" t="s">
-        <v>143</v>
       </c>
       <c r="I16" t="s">
         <v>57</v>
       </c>
       <c r="J16" t="s">
+        <v>143</v>
+      </c>
+      <c r="K16" t="s">
         <v>144</v>
       </c>
-      <c r="K16" t="s">
+      <c r="L16" t="s">
         <v>145</v>
       </c>
-      <c r="L16" t="s">
-        <v>146</v>
-      </c>
       <c r="M16" t="s">
+        <v>147</v>
+      </c>
+      <c r="N16" t="s">
         <v>148</v>
-      </c>
-      <c r="N16" t="s">
-        <v>149</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.2">
@@ -29254,7 +29269,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0732F100-BA00-6B40-9214-8DA7980541D2}">
   <dimension ref="A1:I17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="60" zoomScaleSheetLayoutView="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="60" zoomScaleSheetLayoutView="100" workbookViewId="0">
       <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
@@ -29265,21 +29280,21 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C1" t="s">
         <v>87</v>
       </c>
       <c r="D1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C2">
         <v>30</v>
@@ -29298,10 +29313,10 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C3">
         <v>30</v>
@@ -29324,10 +29339,10 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C4">
         <v>0</v>
@@ -29350,10 +29365,10 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C5">
         <v>0</v>
@@ -29368,18 +29383,18 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B6" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B7" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D7">
         <v>70.42</v>
@@ -29395,10 +29410,10 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B8" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D8">
         <v>141.63999999999999</v>
@@ -29406,18 +29421,18 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B9" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B10" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D10">
         <v>37.42</v>
@@ -29436,7 +29451,7 @@
         <v>91</v>
       </c>
       <c r="B11" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D11">
         <v>177.31</v>
@@ -29447,23 +29462,23 @@
         <v>89</v>
       </c>
       <c r="B12" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B13" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B14" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="F14" t="s">
         <v>27</v>
@@ -29499,8 +29514,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9CBD11D3-C52D-2E44-9DCD-36B6FFFDB589}">
   <dimension ref="A1:D144"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="60" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="D36" sqref="D36"/>
+    <sheetView tabSelected="1" zoomScaleNormal="60" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -29511,13 +29526,13 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B1" t="s">
         <v>87</v>
       </c>
       <c r="C1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D1" t="s">
         <v>6</v>
@@ -29644,7 +29659,7 @@
         <v>5.6101522283700828E-2</v>
       </c>
       <c r="C9" t="s">
-        <v>92</v>
+        <v>149</v>
       </c>
       <c r="D9">
         <f>Table9[[#This Row],[unnorm_x]]-A8</f>
@@ -29708,7 +29723,7 @@
         <v>8.2941063121094505E-2</v>
       </c>
       <c r="C13" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D13">
         <f>Table9[[#This Row],[unnorm_x]]-A12</f>
@@ -29836,7 +29851,7 @@
         <v>0.14039144438021306</v>
       </c>
       <c r="C21" t="s">
-        <v>92</v>
+        <v>150</v>
       </c>
       <c r="D21">
         <f>Table9[[#This Row],[unnorm_x]]-A20</f>
@@ -29900,7 +29915,7 @@
         <v>0.16709334654664576</v>
       </c>
       <c r="C25" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D25">
         <f>Table9[[#This Row],[unnorm_x]]-A24</f>
@@ -30028,7 +30043,7 @@
         <v>0.22528697662895369</v>
       </c>
       <c r="C33" t="s">
-        <v>92</v>
+        <v>151</v>
       </c>
       <c r="D33">
         <f>Table9[[#This Row],[unnorm_x]]-A32</f>
@@ -30092,7 +30107,7 @@
         <v>0.25300740496049773</v>
       </c>
       <c r="C37" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D37">
         <f>Table9[[#This Row],[unnorm_x]]-A36</f>
@@ -30220,7 +30235,7 @@
         <v>0.31067800809315388</v>
       </c>
       <c r="C45" t="s">
-        <v>92</v>
+        <v>152</v>
       </c>
       <c r="D45">
         <f>Table9[[#This Row],[unnorm_x]]-A44</f>
@@ -30284,7 +30299,7 @@
         <v>0.33765518760150853</v>
       </c>
       <c r="C49" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D49">
         <f>Table9[[#This Row],[unnorm_x]]-A48</f>
@@ -30412,7 +30427,7 @@
         <v>0.39513309659481927</v>
       </c>
       <c r="C57" t="s">
-        <v>92</v>
+        <v>153</v>
       </c>
       <c r="D57">
         <f>Table9[[#This Row],[unnorm_x]]-A56</f>
@@ -30476,7 +30491,7 @@
         <v>0.42211027610317398</v>
       </c>
       <c r="C61" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D61">
         <f>Table9[[#This Row],[unnorm_x]]-A60</f>
@@ -30604,7 +30619,7 @@
         <v>0.48019379524871308</v>
       </c>
       <c r="C69" t="s">
-        <v>92</v>
+        <v>154</v>
       </c>
       <c r="D69">
         <f>Table9[[#This Row],[unnorm_x]]-A68</f>
@@ -30668,7 +30683,7 @@
         <v>0.5065928923390316</v>
       </c>
       <c r="C73" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D73">
         <f>Table9[[#This Row],[unnorm_x]]-A72</f>
@@ -30796,7 +30811,7 @@
         <v>0.56407080133234233</v>
       </c>
       <c r="C81" t="s">
-        <v>92</v>
+        <v>154</v>
       </c>
       <c r="D81">
         <f>Table9[[#This Row],[unnorm_x]]-A80</f>
@@ -30860,7 +30875,7 @@
         <v>0.59115809177746581</v>
       </c>
       <c r="C85" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D85">
         <f>Table9[[#This Row],[unnorm_x]]-A84</f>
@@ -30988,7 +31003,7 @@
         <v>0.6487736394417376</v>
       </c>
       <c r="C93" t="s">
-        <v>92</v>
+        <v>154</v>
       </c>
       <c r="D93">
         <f>Table9[[#This Row],[unnorm_x]]-A92</f>
@@ -31052,7 +31067,7 @@
         <v>0.67583340215266885</v>
       </c>
       <c r="C97" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D97">
         <f>Table9[[#This Row],[unnorm_x]]-A96</f>
@@ -31116,7 +31131,7 @@
         <v>0.70181958323010429</v>
       </c>
       <c r="C101" t="s">
-        <v>92</v>
+        <v>152</v>
       </c>
       <c r="D101">
         <f>Table9[[#This Row],[unnorm_x]]-A100</f>
@@ -31244,7 +31259,7 @@
         <v>0.76004074104660457</v>
       </c>
       <c r="C109" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D109">
         <f>Table9[[#This Row],[unnorm_x]]-A108</f>
@@ -31308,7 +31323,7 @@
         <v>0.78624714399757756</v>
       </c>
       <c r="C113" t="s">
-        <v>92</v>
+        <v>151</v>
       </c>
       <c r="D113">
         <f>Table9[[#This Row],[unnorm_x]]-A112</f>
@@ -31436,7 +31451,7 @@
         <v>0.8447160514218075</v>
       </c>
       <c r="C121" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D121">
         <f>Table9[[#This Row],[unnorm_x]]-A120</f>
@@ -31500,7 +31515,7 @@
         <v>0.87083987117020412</v>
       </c>
       <c r="C125" t="s">
-        <v>92</v>
+        <v>150</v>
       </c>
       <c r="D125">
         <f>Table9[[#This Row],[unnorm_x]]-A124</f>
@@ -31628,7 +31643,7 @@
         <v>0.92941888953120277</v>
       </c>
       <c r="C133" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D133">
         <f>Table9[[#This Row],[unnorm_x]]-A132</f>
@@ -31692,7 +31707,7 @@
         <v>0.95570787568475246</v>
       </c>
       <c r="C137" t="s">
-        <v>92</v>
+        <v>149</v>
       </c>
       <c r="D137">
         <f>Table9[[#This Row],[unnorm_x]]-A136</f>

</xml_diff>